<commit_message>
Testing encoding msg to 15 coefs.
</commit_message>
<xml_diff>
--- a/code/PSNR-result/kok.xlsx
+++ b/code/PSNR-result/kok.xlsx
@@ -22,6 +22,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
+    <t xml:space="preserve">PSNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chromosome</t>
+  </si>
+  <si>
     <t xml:space="preserve">0 1 1 1 0 1 0 1 1 0 </t>
   </si>
   <si>
@@ -55,9 +61,6 @@
     <t xml:space="preserve">1 1 1 0 0 1 1 1 0 0 </t>
   </si>
   <si>
-    <t xml:space="preserve">1 1 1 1 1 0 1 0 0 1 </t>
-  </si>
-  <si>
     <t xml:space="preserve">0 1 0 1 0 0 1 1 1 1 </t>
   </si>
   <si>
@@ -83,17 +86,15 @@
   </si>
   <si>
     <t xml:space="preserve">1 1 0 0 1 0 1 1 0 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">33.287957994937386</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -163,8 +164,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -177,15 +190,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -194,191 +198,199 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
         <v>32.9338720319804</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
         <v>33.0153881883192</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
         <v>33.0632287708516</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
         <v>33.1653001254655</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
         <v>33.2035495803442</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
         <v>33.2559514700976</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
         <v>33.258959843139</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
         <v>33.2933921428772</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
         <v>33.3128901482205</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
         <v>33.3143597900676</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
         <v>33.3868456583612</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>33.436256811598</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>11</v>
+      <c r="B12" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="2" t="n">
         <v>33.5443759494224</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>12</v>
+      <c r="B13" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="2" t="n">
         <v>33.54458788089</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>13</v>
+      <c r="B14" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="2" t="n">
         <v>33.7036899638696</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>14</v>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="2" t="n">
         <v>33.7136894115217</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>15</v>
+      <c r="B16" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="2" t="n">
         <v>33.7796587344963</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>16</v>
+      <c r="B17" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="2" t="n">
         <v>33.8339976024475</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>17</v>
+      <c r="B18" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="2" t="n">
         <v>33.9103330596288</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>18</v>
+      <c r="B19" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="2" t="n">
         <v>33.9215389872142</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>19</v>
+      <c r="B20" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="2" t="n">
         <v>33.9832628455876</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="0" t="s">
+      <c r="B21" s="3" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:B21">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>